<commit_message>
Initial Test ok and some adjustments
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vibar\source\repos\Grading_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E50ACE5B-BE49-4E0E-BFC0-6DE3274D8C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E64727-5AAC-4DAC-9619-9498C22EFE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5556E41F-37F1-4019-B9F4-E20A2B8CE86F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="57">
   <si>
     <t>Duran</t>
   </si>
@@ -183,6 +183,30 @@
   </si>
   <si>
     <t>Female</t>
+  </si>
+  <si>
+    <t>Saragpon, Daniel Catequista</t>
+  </si>
+  <si>
+    <t>Vibar, Miles Dominic Morales</t>
+  </si>
+  <si>
+    <t>Rizal</t>
+  </si>
+  <si>
+    <t>Shakespeare</t>
+  </si>
+  <si>
+    <t>Industrious</t>
+  </si>
+  <si>
+    <t>Perseverance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Noa, Kenji Isaac </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zurbano, Christopher Ian </t>
   </si>
 </sst>
 </file>
@@ -218,8 +242,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,15 +567,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{618455EF-5A7C-4D04-83D3-6F8BF5710847}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,11 +597,18 @@
         <f>10000+1</f>
         <v>10001</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -580,11 +625,18 @@
         <f>E1+1</f>
         <v>10002</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -601,11 +653,18 @@
         <f t="shared" ref="E3:E20" si="0">E2+1</f>
         <v>10003</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -622,11 +681,18 @@
         <f t="shared" si="0"/>
         <v>10004</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -643,11 +709,17 @@
         <f t="shared" si="0"/>
         <v>10005</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -664,11 +736,17 @@
         <f t="shared" si="0"/>
         <v>10006</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -685,11 +763,17 @@
         <f t="shared" si="0"/>
         <v>10007</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -706,11 +790,17 @@
         <f t="shared" si="0"/>
         <v>10008</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -727,11 +817,17 @@
         <f t="shared" si="0"/>
         <v>10009</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -748,11 +844,17 @@
         <f t="shared" si="0"/>
         <v>10010</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -769,11 +871,17 @@
         <f t="shared" si="0"/>
         <v>10011</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -790,11 +898,17 @@
         <f t="shared" si="0"/>
         <v>10012</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -811,11 +925,17 @@
         <f t="shared" si="0"/>
         <v>10013</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -832,11 +952,17 @@
         <f t="shared" si="0"/>
         <v>10014</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H14">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -853,11 +979,17 @@
         <f t="shared" si="0"/>
         <v>10015</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -874,11 +1006,17 @@
         <f t="shared" si="0"/>
         <v>10016</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -895,11 +1033,17 @@
         <f t="shared" si="0"/>
         <v>10017</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -916,11 +1060,17 @@
         <f t="shared" si="0"/>
         <v>10018</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -937,11 +1087,17 @@
         <f t="shared" si="0"/>
         <v>10019</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -958,7 +1114,13 @@
         <f t="shared" si="0"/>
         <v>10020</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20">
         <v>4</v>
       </c>
     </row>

</xml_diff>